<commit_message>
use simulated energy/nutrient recoveries and user cost
</commit_message>
<xml_diff>
--- a/dmsan/data/bwaise_uncertainties.xlsx
+++ b/dmsan/data/bwaise_uncertainties.xlsx
@@ -528,46 +528,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.09466344414961556</v>
+        <v>0.1342738309092486</v>
       </c>
       <c r="C4">
-        <v>0.02136785336183554</v>
+        <v>0.3068946229648429</v>
       </c>
       <c r="D4">
-        <v>0.1699496944694366</v>
+        <v>0.3792738958163777</v>
       </c>
       <c r="E4">
-        <v>0.09126903862188955</v>
+        <v>0.7699587499801355</v>
       </c>
       <c r="F4">
-        <v>8.234793826277203</v>
+        <v>9.02213093779962</v>
       </c>
       <c r="G4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="H4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="I4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="J4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="K4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="L4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="M4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="N4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
       <c r="O4">
-        <v>0.3805820671604604</v>
+        <v>-0.01227840136682937</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -575,46 +575,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.1205572545800305</v>
+        <v>0.117102317617044</v>
       </c>
       <c r="C5">
-        <v>0.009900164663814791</v>
+        <v>0.3351565768944674</v>
       </c>
       <c r="D5">
-        <v>0.1235964428284451</v>
+        <v>0.453289065124413</v>
       </c>
       <c r="E5">
-        <v>0.1349327208183131</v>
+        <v>0.8101987431425259</v>
       </c>
       <c r="F5">
-        <v>14.25690047516862</v>
+        <v>7.533521445093559</v>
       </c>
       <c r="G5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="H5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="I5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="J5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="K5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="L5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="M5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="N5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
       <c r="O5">
-        <v>0.586366636358191</v>
+        <v>-0.170343031747453</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -622,46 +622,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.09595487722403878</v>
+        <v>0.160772655053185</v>
       </c>
       <c r="C6">
-        <v>0.01604460563620833</v>
+        <v>0.2580955683666594</v>
       </c>
       <c r="D6">
-        <v>0.2232385494057853</v>
+        <v>0.4909121338760611</v>
       </c>
       <c r="E6">
-        <v>0.1699588363338861</v>
+        <v>0.6890321352291153</v>
       </c>
       <c r="F6">
-        <v>10.7825781140121</v>
+        <v>12.69350852898792</v>
       </c>
       <c r="G6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="H6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="I6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="J6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="K6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="L6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="M6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="N6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
       <c r="O6">
-        <v>0.4027847994156919</v>
+        <v>0.2500308114812562</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -669,46 +669,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.1403016061431178</v>
+        <v>0.1569576065510177</v>
       </c>
       <c r="C7">
-        <v>0.006398170464545684</v>
+        <v>0.3223550273928166</v>
       </c>
       <c r="D7">
-        <v>0.09348634301269</v>
+        <v>0.378817047317041</v>
       </c>
       <c r="E7">
-        <v>0.1047732881723575</v>
+        <v>0.8049342107922487</v>
       </c>
       <c r="F7">
-        <v>8.433921080387064</v>
+        <v>6.356010523647634</v>
       </c>
       <c r="G7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="H7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="I7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="J7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="K7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="L7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="M7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="N7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
       <c r="O7">
-        <v>0.1752532604718951</v>
+        <v>-0.1236371152028135</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -716,46 +716,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.1361003816920413</v>
+        <v>0.1455960473375892</v>
       </c>
       <c r="C8">
-        <v>0.01331690485036441</v>
+        <v>0.1950090363444807</v>
       </c>
       <c r="D8">
-        <v>0.2044908061965185</v>
+        <v>0.321228798040022</v>
       </c>
       <c r="E8">
-        <v>0.147577615818088</v>
+        <v>0.7952780612303839</v>
       </c>
       <c r="F8">
-        <v>12.28129821672621</v>
+        <v>5.096615143188213</v>
       </c>
       <c r="G8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="H8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="I8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="J8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="K8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="L8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="M8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="N8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
       <c r="O8">
-        <v>0.4310758088761051</v>
+        <v>-0.103423759704236</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -763,46 +763,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.1200532303689134</v>
+        <v>0.1808861351969999</v>
       </c>
       <c r="C9">
-        <v>0.01295878354642125</v>
+        <v>0.2721785279931249</v>
       </c>
       <c r="D9">
-        <v>0.2154165747677679</v>
+        <v>0.5283451055459296</v>
       </c>
       <c r="E9">
-        <v>0.1061988158500689</v>
+        <v>0.8611017209833431</v>
       </c>
       <c r="F9">
-        <v>6.180017783282887</v>
+        <v>12.12759738260616</v>
       </c>
       <c r="G9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="H9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="I9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="J9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="K9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="L9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="M9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="N9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
       <c r="O9">
-        <v>0.1094151189772857</v>
+        <v>0.02889987754234994</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -810,46 +810,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.1034191984255462</v>
+        <v>0.1397922558554177</v>
       </c>
       <c r="C10">
-        <v>0.01465024475232964</v>
+        <v>0.3047910267842072</v>
       </c>
       <c r="D10">
-        <v>0.2161425199055692</v>
+        <v>0.4205772433913187</v>
       </c>
       <c r="E10">
-        <v>0.09171383131411634</v>
+        <v>0.7201330704907718</v>
       </c>
       <c r="F10">
-        <v>7.674018909869686</v>
+        <v>19.50412435053004</v>
       </c>
       <c r="G10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="H10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="I10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="J10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="K10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="L10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="M10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="N10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
       <c r="O10">
-        <v>0.1657193427928853</v>
+        <v>0.2838249703872437</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -857,46 +857,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.1147144088747248</v>
+        <v>0.1063380514765014</v>
       </c>
       <c r="C11">
-        <v>0.008828636360300662</v>
+        <v>0.3294580012685623</v>
       </c>
       <c r="D11">
-        <v>0.1743204189768876</v>
+        <v>0.4207683533692542</v>
       </c>
       <c r="E11">
-        <v>0.181873142017669</v>
+        <v>0.6930348321901609</v>
       </c>
       <c r="F11">
-        <v>9.012746990471673</v>
+        <v>5.230486504387351</v>
       </c>
       <c r="G11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="H11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="I11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="J11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="K11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="L11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="M11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="N11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
       <c r="O11">
-        <v>0.2380078315124876</v>
+        <v>-0.1692097445614708</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -904,46 +904,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.1707691176853539</v>
+        <v>0.1346241340006396</v>
       </c>
       <c r="C12">
-        <v>0.025711285473725</v>
+        <v>0.2152796917297022</v>
       </c>
       <c r="D12">
-        <v>0.1422627518984698</v>
+        <v>0.5132098620935431</v>
       </c>
       <c r="E12">
-        <v>0.02963508590667179</v>
+        <v>0.759277606170304</v>
       </c>
       <c r="F12">
-        <v>13.46018939364824</v>
+        <v>14.9001726673994</v>
       </c>
       <c r="G12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="H12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="I12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="J12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="K12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="L12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="M12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="N12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
       <c r="O12">
-        <v>0.6109808649177114</v>
+        <v>0.3365780277984713</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -951,46 +951,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.1201178727948516</v>
+        <v>0.1083987181841536</v>
       </c>
       <c r="C13">
-        <v>0.007158397178026462</v>
+        <v>0.2216410511425598</v>
       </c>
       <c r="D13">
-        <v>0.2970416106408074</v>
+        <v>0.3555345617819903</v>
       </c>
       <c r="E13">
-        <v>0.06780466815801246</v>
+        <v>0.7677676499523128</v>
       </c>
       <c r="F13">
-        <v>7.87917485128346</v>
+        <v>6.47495117760737</v>
       </c>
       <c r="G13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="H13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="I13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="J13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="K13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="L13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="M13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="N13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
       <c r="O13">
-        <v>0.240994288081528</v>
+        <v>-0.05561647331730443</v>
       </c>
     </row>
   </sheetData>
@@ -1092,46 +1092,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.5487731178211059</v>
+        <v>0.3404985380793831</v>
       </c>
       <c r="C4">
-        <v>0.5264106562189946</v>
+        <v>0.3236492621527796</v>
       </c>
       <c r="D4">
-        <v>0.7716653556855295</v>
+        <v>0.816612326943446</v>
       </c>
       <c r="E4">
-        <v>0.8033606110507906</v>
+        <v>0.8992486843170349</v>
       </c>
       <c r="F4">
-        <v>8.322126220620408</v>
+        <v>7.11631654777257</v>
       </c>
       <c r="G4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="H4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="I4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="J4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="K4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="L4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="M4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="N4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
       <c r="O4">
-        <v>-0.342151317116768</v>
+        <v>-0.1767951139780164</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1139,46 +1139,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.2677760222425688</v>
+        <v>0.3891958581353412</v>
       </c>
       <c r="C5">
-        <v>0.1635929885957638</v>
+        <v>0.2098505645987911</v>
       </c>
       <c r="D5">
-        <v>0.6986617190398594</v>
+        <v>0.8446827158465987</v>
       </c>
       <c r="E5">
-        <v>0.7212977648019179</v>
+        <v>0.7446006363740362</v>
       </c>
       <c r="F5">
-        <v>7.129444114671685</v>
+        <v>3.920309885524912</v>
       </c>
       <c r="G5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="H5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="I5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="J5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="K5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="L5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="M5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="N5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
       <c r="O5">
-        <v>-0.1612285714962285</v>
+        <v>-0.3280323434485395</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1186,46 +1186,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.3414754798810697</v>
+        <v>0.3647766285496614</v>
       </c>
       <c r="C6">
-        <v>0.2649343976527975</v>
+        <v>0.2672617325075488</v>
       </c>
       <c r="D6">
-        <v>0.6426117630523948</v>
+        <v>0.7629398292744867</v>
       </c>
       <c r="E6">
-        <v>0.866531805984218</v>
+        <v>0.7953010898418792</v>
       </c>
       <c r="F6">
-        <v>10.77440302753268</v>
+        <v>11.58213234698223</v>
       </c>
       <c r="G6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="H6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="I6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="J6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="K6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="L6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="M6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="N6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
       <c r="O6">
-        <v>0.233090830536971</v>
+        <v>-0.08576727761679209</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1233,46 +1233,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.3216299361636158</v>
+        <v>0.397692802485008</v>
       </c>
       <c r="C7">
-        <v>0.2430095539561905</v>
+        <v>0.3091803690571324</v>
       </c>
       <c r="D7">
-        <v>0.8814977424139918</v>
+        <v>0.6830149595163397</v>
       </c>
       <c r="E7">
-        <v>0.7207742816728395</v>
+        <v>0.6767220319780584</v>
       </c>
       <c r="F7">
-        <v>8.275510688311039</v>
+        <v>8.845353267439352</v>
       </c>
       <c r="G7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="H7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="I7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="J7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="K7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="L7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="M7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="N7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
       <c r="O7">
-        <v>-0.07436985318514769</v>
+        <v>-0.06506959985698424</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1280,46 +1280,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.4046258233295913</v>
+        <v>0.4598475553701047</v>
       </c>
       <c r="C8">
-        <v>0.2886346022178893</v>
+        <v>0.2032479242674561</v>
       </c>
       <c r="D8">
-        <v>0.8614756860078604</v>
+        <v>0.9199982404493721</v>
       </c>
       <c r="E8">
-        <v>0.716321492679566</v>
+        <v>0.778201008798621</v>
       </c>
       <c r="F8">
-        <v>3.394935303392531</v>
+        <v>3.130703678760561</v>
       </c>
       <c r="G8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="H8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="I8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="J8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="K8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="L8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="M8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="N8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
       <c r="O8">
-        <v>-0.373939039924408</v>
+        <v>-0.4088725084040999</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1327,46 +1327,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.5406987050024606</v>
+        <v>0.4145230477637146</v>
       </c>
       <c r="C9">
-        <v>0.412446667837172</v>
+        <v>0.3332279073387567</v>
       </c>
       <c r="D9">
-        <v>0.6707220659852626</v>
+        <v>0.8474797462352981</v>
       </c>
       <c r="E9">
-        <v>0.7885829716491475</v>
+        <v>0.7401643063544607</v>
       </c>
       <c r="F9">
-        <v>3.976086461187507</v>
+        <v>18.89730183370705</v>
       </c>
       <c r="G9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="H9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="I9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="J9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="K9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="L9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="M9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="N9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
       <c r="O9">
-        <v>-0.3682928091900218</v>
+        <v>0.3738936816160691</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1374,46 +1374,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.3039582596097705</v>
+        <v>0.3730301435559069</v>
       </c>
       <c r="C10">
-        <v>0.1479771157704783</v>
+        <v>0.2114050728472736</v>
       </c>
       <c r="D10">
-        <v>0.7006572641744351</v>
+        <v>0.7653985127840373</v>
       </c>
       <c r="E10">
-        <v>0.6742344807681678</v>
+        <v>0.7534390211370979</v>
       </c>
       <c r="F10">
-        <v>13.34286967106047</v>
+        <v>13.65092825240612</v>
       </c>
       <c r="G10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="H10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="I10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="J10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="K10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="L10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="M10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="N10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
       <c r="O10">
-        <v>0.6014790651110957</v>
+        <v>0.1481157120954539</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1421,46 +1421,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.3762930370461904</v>
+        <v>0.3785693436802047</v>
       </c>
       <c r="C11">
-        <v>0.2770125054360976</v>
+        <v>0.3371721402770567</v>
       </c>
       <c r="D11">
-        <v>0.6935214585427745</v>
+        <v>0.6264017169442121</v>
       </c>
       <c r="E11">
-        <v>0.7099387488191037</v>
+        <v>0.7661602120379316</v>
       </c>
       <c r="F11">
-        <v>5.962195031961366</v>
+        <v>7.385832721835889</v>
       </c>
       <c r="G11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="H11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="I11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="J11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="K11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="L11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="M11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="N11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
       <c r="O11">
-        <v>-0.2248919521474852</v>
+        <v>-0.06902148237131539</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1468,46 +1468,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.3409226809330815</v>
+        <v>0.2540470619189764</v>
       </c>
       <c r="C12">
-        <v>0.2498766912690933</v>
+        <v>0.250001203637881</v>
       </c>
       <c r="D12">
-        <v>0.874877020255866</v>
+        <v>0.8305448115271902</v>
       </c>
       <c r="E12">
-        <v>0.7390552283632658</v>
+        <v>0.6232225847835118</v>
       </c>
       <c r="F12">
-        <v>5.499093927763234</v>
+        <v>6.172087277874474</v>
       </c>
       <c r="G12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="H12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="I12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="J12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="K12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="L12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="M12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="N12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
       <c r="O12">
-        <v>-0.1843163017959865</v>
+        <v>-0.1436852634511429</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1515,46 +1515,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.5341080209744709</v>
+        <v>0.4743048217246052</v>
       </c>
       <c r="C13">
-        <v>0.3445456620326878</v>
+        <v>0.2959430403925805</v>
       </c>
       <c r="D13">
-        <v>0.9319818248756981</v>
+        <v>0.6233774972129159</v>
       </c>
       <c r="E13">
-        <v>0.7312970407484569</v>
+        <v>0.6951953230935235</v>
       </c>
       <c r="F13">
-        <v>17.96987627655681</v>
+        <v>6.809589567074502</v>
       </c>
       <c r="G13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="H13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="I13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="J13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="K13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="L13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="M13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="N13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
       <c r="O13">
-        <v>0.5653928419316935</v>
+        <v>-0.2308484305895594</v>
       </c>
     </row>
   </sheetData>
@@ -1656,46 +1656,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.4002171391590728</v>
+        <v>0.4813036000497379</v>
       </c>
       <c r="C4">
-        <v>0.06634311095940923</v>
+        <v>0.8669464909990061</v>
       </c>
       <c r="D4">
-        <v>0.4693487238614814</v>
+        <v>0.6047327411485997</v>
       </c>
       <c r="E4">
-        <v>0.2428703961256102</v>
+        <v>0.9883575771379397</v>
       </c>
       <c r="F4">
-        <v>29.93749029250896</v>
+        <v>21.97777617341347</v>
       </c>
       <c r="G4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="H4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="I4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="J4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="K4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="L4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="M4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="N4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
       <c r="O4">
-        <v>0.7565576850474961</v>
+        <v>0.08855165436982884</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1703,46 +1703,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.4780486235837795</v>
+        <v>0.49281065566889</v>
       </c>
       <c r="C5">
-        <v>0.0486302547878991</v>
+        <v>0.8125204316230247</v>
       </c>
       <c r="D5">
-        <v>0.4561364041079543</v>
+        <v>0.6599481343843909</v>
       </c>
       <c r="E5">
-        <v>0.3810396575367854</v>
+        <v>0.9212110695789697</v>
       </c>
       <c r="F5">
-        <v>49.4036040276839</v>
+        <v>35.09304065811545</v>
       </c>
       <c r="G5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="H5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="I5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="J5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="K5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="L5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="M5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="N5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
       <c r="O5">
-        <v>4.865470882954504</v>
+        <v>0.3468738891874102</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1750,46 +1750,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.5066504881770969</v>
+        <v>0.5010986894508617</v>
       </c>
       <c r="C6">
-        <v>0.08423620418552887</v>
+        <v>0.8647140272499581</v>
       </c>
       <c r="D6">
-        <v>0.5588015040758652</v>
+        <v>0.627656899670919</v>
       </c>
       <c r="E6">
-        <v>0.3540685597494086</v>
+        <v>0.9683446984132138</v>
       </c>
       <c r="F6">
-        <v>38.71212975592508</v>
+        <v>38.56710507158374</v>
       </c>
       <c r="G6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="H6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="I6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="J6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="K6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="L6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="M6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="N6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
       <c r="O6">
-        <v>1.192899678153523</v>
+        <v>0.5828316123693374</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1797,46 +1797,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.4574193424163731</v>
+        <v>0.5568973137503673</v>
       </c>
       <c r="C7">
-        <v>0.1224560081296371</v>
+        <v>0.859035605326836</v>
       </c>
       <c r="D7">
-        <v>0.5940277726264098</v>
+        <v>0.6717793388374531</v>
       </c>
       <c r="E7">
-        <v>0.208379393677763</v>
+        <v>0.9861119698266072</v>
       </c>
       <c r="F7">
-        <v>37.33131397268498</v>
+        <v>38.26032941225483</v>
       </c>
       <c r="G7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="H7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="I7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="J7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="K7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="L7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="M7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="N7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
       <c r="O7">
-        <v>0.6187507837617621</v>
+        <v>1.254216328613806</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1844,46 +1844,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.4342342278968712</v>
+        <v>0.4510100136757352</v>
       </c>
       <c r="C8">
-        <v>0.05733751985448893</v>
+        <v>0.8389653843801657</v>
       </c>
       <c r="D8">
-        <v>0.278270972924856</v>
+        <v>0.616546371201895</v>
       </c>
       <c r="E8">
-        <v>0.08405008154128732</v>
+        <v>0.9891135969256521</v>
       </c>
       <c r="F8">
-        <v>51.17092123364915</v>
+        <v>26.29207472298372</v>
       </c>
       <c r="G8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="H8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="I8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="J8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="K8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="L8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="M8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="N8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
       <c r="O8">
-        <v>2.941877916422404</v>
+        <v>0.5208117114527848</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1891,46 +1891,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.4836018556384092</v>
+        <v>0.4012507430652762</v>
       </c>
       <c r="C9">
-        <v>0.05554964833302323</v>
+        <v>0.8372111617839993</v>
       </c>
       <c r="D9">
-        <v>0.4493424261508286</v>
+        <v>0.6009484894043411</v>
       </c>
       <c r="E9">
-        <v>0.2653561882163394</v>
+        <v>0.9827482295720914</v>
       </c>
       <c r="F9">
-        <v>29.02166925215167</v>
+        <v>42.92192830022178</v>
       </c>
       <c r="G9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="H9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="I9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="J9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="K9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="L9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="M9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="N9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
       <c r="O9">
-        <v>1.504341733604643</v>
+        <v>0.6147259615237898</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1938,46 +1938,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.4590494854726135</v>
+        <v>0.533681084688559</v>
       </c>
       <c r="C10">
-        <v>0.08074067609521605</v>
+        <v>0.7995682964875506</v>
       </c>
       <c r="D10">
-        <v>0.3293779928108362</v>
+        <v>0.6236034439428224</v>
       </c>
       <c r="E10">
-        <v>0.1781199892602487</v>
+        <v>0.982711461085473</v>
       </c>
       <c r="F10">
-        <v>24.87668931958557</v>
+        <v>34.18852041523162</v>
       </c>
       <c r="G10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="H10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="I10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="J10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="K10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="L10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="M10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="N10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
       <c r="O10">
-        <v>1.332215428861376</v>
+        <v>0.1770869208847956</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1985,46 +1985,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.4686462493743766</v>
+        <v>0.5339219698899847</v>
       </c>
       <c r="C11">
-        <v>0.07459031745925472</v>
+        <v>0.8261299281310026</v>
       </c>
       <c r="D11">
-        <v>0.4060790098158547</v>
+        <v>0.57526470341659</v>
       </c>
       <c r="E11">
-        <v>0.3341820217007868</v>
+        <v>0.9531485199903575</v>
       </c>
       <c r="F11">
-        <v>40.0409133599427</v>
+        <v>69.83362817448757</v>
       </c>
       <c r="G11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="H11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="I11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="J11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="K11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="L11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="M11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="N11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
       <c r="O11">
-        <v>2.705083374023978</v>
+        <v>6.301488134964102</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -2032,46 +2032,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.5492725340961193</v>
+        <v>0.51853711896593</v>
       </c>
       <c r="C12">
-        <v>0.1014086638708405</v>
+        <v>0.8710800683111276</v>
       </c>
       <c r="D12">
-        <v>0.3783307474494817</v>
+        <v>0.6264029431560781</v>
       </c>
       <c r="E12">
-        <v>0.2916786363778789</v>
+        <v>1.032854135276037</v>
       </c>
       <c r="F12">
-        <v>29.59493154998936</v>
+        <v>31.94571874549643</v>
       </c>
       <c r="G12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="H12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="I12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="J12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="K12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="L12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="M12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="N12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
       <c r="O12">
-        <v>0.8137032379550111</v>
+        <v>3.42947309439512</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2079,46 +2079,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.5081989879214743</v>
+        <v>0.4066424522202957</v>
       </c>
       <c r="C13">
-        <v>0.1143074506995858</v>
+        <v>0.8159884965488076</v>
       </c>
       <c r="D13">
-        <v>0.411169925912946</v>
+        <v>0.4871506396883109</v>
       </c>
       <c r="E13">
-        <v>0.2433471853953777</v>
+        <v>0.9714380511667401</v>
       </c>
       <c r="F13">
-        <v>75.0307196875815</v>
+        <v>41.88085624618613</v>
       </c>
       <c r="G13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="H13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="I13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="J13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="K13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="L13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="M13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="N13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
       <c r="O13">
-        <v>5.791072476325976</v>
+        <v>1.685553353225906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update energy recovery calculation
</commit_message>
<xml_diff>
--- a/dmsan/data/bwaise_uncertainties.xlsx
+++ b/dmsan/data/bwaise_uncertainties.xlsx
@@ -528,46 +528,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.1342738309092486</v>
+        <v>0.1858085114967375</v>
       </c>
       <c r="C4">
-        <v>0.3068946229648429</v>
+        <v>0.3563072026057131</v>
       </c>
       <c r="D4">
-        <v>0.3792738958163777</v>
+        <v>0.5919561851532162</v>
       </c>
       <c r="E4">
-        <v>0.7699587499801355</v>
+        <v>0.7771935300218524</v>
       </c>
       <c r="F4">
-        <v>9.02213093779962</v>
+        <v>25.18947145510401</v>
       </c>
       <c r="G4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="H4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="I4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="J4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="K4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="L4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="M4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="N4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
       <c r="O4">
-        <v>-0.01227840136682937</v>
+        <v>0.625740982600542</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -575,46 +575,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.117102317617044</v>
+        <v>0.1798846390951423</v>
       </c>
       <c r="C5">
-        <v>0.3351565768944674</v>
+        <v>0.4413242135561269</v>
       </c>
       <c r="D5">
-        <v>0.453289065124413</v>
+        <v>0.4310668614703931</v>
       </c>
       <c r="E5">
-        <v>0.8101987431425259</v>
+        <v>0.851439465624896</v>
       </c>
       <c r="F5">
-        <v>7.533521445093559</v>
+        <v>6.877471575877322</v>
       </c>
       <c r="G5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="H5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="I5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="J5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="K5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="L5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="M5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="N5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
       <c r="O5">
-        <v>-0.170343031747453</v>
+        <v>-0.1473806815676765</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -622,46 +622,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.160772655053185</v>
+        <v>0.1618184817250657</v>
       </c>
       <c r="C6">
-        <v>0.2580955683666594</v>
+        <v>0.1679402863770916</v>
       </c>
       <c r="D6">
-        <v>0.4909121338760611</v>
+        <v>0.3817461055599691</v>
       </c>
       <c r="E6">
-        <v>0.6890321352291153</v>
+        <v>0.8645065030623683</v>
       </c>
       <c r="F6">
-        <v>12.69350852898792</v>
+        <v>5.371641588120073</v>
       </c>
       <c r="G6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="H6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="I6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="J6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="K6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="L6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="M6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="N6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
       <c r="O6">
-        <v>0.2500308114812562</v>
+        <v>-0.005639627271716906</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -669,46 +669,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.1569576065510177</v>
+        <v>0.1186134511861995</v>
       </c>
       <c r="C7">
-        <v>0.3223550273928166</v>
+        <v>0.2858153476448704</v>
       </c>
       <c r="D7">
-        <v>0.378817047317041</v>
+        <v>0.3907698212827988</v>
       </c>
       <c r="E7">
-        <v>0.8049342107922487</v>
+        <v>0.7153988449759283</v>
       </c>
       <c r="F7">
-        <v>6.356010523647634</v>
+        <v>13.05304729947542</v>
       </c>
       <c r="G7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="H7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="I7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="J7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="K7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="L7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="M7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="N7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
       <c r="O7">
-        <v>-0.1236371152028135</v>
+        <v>0.1458753259013291</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -716,46 +716,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.1455960473375892</v>
+        <v>0.1074433978018988</v>
       </c>
       <c r="C8">
-        <v>0.1950090363444807</v>
+        <v>0.1605229374800936</v>
       </c>
       <c r="D8">
-        <v>0.321228798040022</v>
+        <v>0.3805894782034044</v>
       </c>
       <c r="E8">
-        <v>0.7952780612303839</v>
+        <v>0.7380040561185967</v>
       </c>
       <c r="F8">
-        <v>5.096615143188213</v>
+        <v>8.505230636165336</v>
       </c>
       <c r="G8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="H8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="I8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="J8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="K8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="L8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="M8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="N8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
       <c r="O8">
-        <v>-0.103423759704236</v>
+        <v>-0.02316381448275251</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -763,46 +763,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.1808861351969999</v>
+        <v>0.1576530055630601</v>
       </c>
       <c r="C9">
-        <v>0.2721785279931249</v>
+        <v>0.3456990255859899</v>
       </c>
       <c r="D9">
-        <v>0.5283451055459296</v>
+        <v>0.329547650891554</v>
       </c>
       <c r="E9">
-        <v>0.8611017209833431</v>
+        <v>0.6334332959728893</v>
       </c>
       <c r="F9">
-        <v>12.12759738260616</v>
+        <v>7.018911968757545</v>
       </c>
       <c r="G9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="H9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="I9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="J9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="K9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="L9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="M9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="N9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
       <c r="O9">
-        <v>0.02889987754234994</v>
+        <v>-0.1292299507638267</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -810,46 +810,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.1397922558554177</v>
+        <v>0.1454584287340857</v>
       </c>
       <c r="C10">
-        <v>0.3047910267842072</v>
+        <v>0.2438721941082342</v>
       </c>
       <c r="D10">
-        <v>0.4205772433913187</v>
+        <v>0.4592338083180597</v>
       </c>
       <c r="E10">
-        <v>0.7201330704907718</v>
+        <v>0.7763515604990767</v>
       </c>
       <c r="F10">
-        <v>19.50412435053004</v>
+        <v>4.203094245986535</v>
       </c>
       <c r="G10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="H10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="I10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="J10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="K10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="L10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="M10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="N10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
       <c r="O10">
-        <v>0.2838249703872437</v>
+        <v>-0.1528105898376427</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -857,46 +857,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.1063380514765014</v>
+        <v>0.1111278833498997</v>
       </c>
       <c r="C11">
-        <v>0.3294580012685623</v>
+        <v>0.2531732803482239</v>
       </c>
       <c r="D11">
-        <v>0.4207683533692542</v>
+        <v>0.4139325603720986</v>
       </c>
       <c r="E11">
-        <v>0.6930348321901609</v>
+        <v>0.796920612350297</v>
       </c>
       <c r="F11">
-        <v>5.230486504387351</v>
+        <v>8.526739196153407</v>
       </c>
       <c r="G11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="H11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="I11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="J11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="K11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="L11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="M11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="N11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
       <c r="O11">
-        <v>-0.1692097445614708</v>
+        <v>0.02081426167297521</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -904,46 +904,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.1346241340006396</v>
+        <v>0.1114144019445487</v>
       </c>
       <c r="C12">
-        <v>0.2152796917297022</v>
+        <v>0.3015371328012756</v>
       </c>
       <c r="D12">
-        <v>0.5132098620935431</v>
+        <v>0.429122988244345</v>
       </c>
       <c r="E12">
-        <v>0.759277606170304</v>
+        <v>0.8373274856745683</v>
       </c>
       <c r="F12">
-        <v>14.9001726673994</v>
+        <v>14.02496213864898</v>
       </c>
       <c r="G12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="H12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="I12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="J12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="K12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="L12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="M12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="N12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
       <c r="O12">
-        <v>0.3365780277984713</v>
+        <v>0.242359568136641</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -951,46 +951,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.1083987181841536</v>
+        <v>0.1325190190826571</v>
       </c>
       <c r="C13">
-        <v>0.2216410511425598</v>
+        <v>0.3081912616437623</v>
       </c>
       <c r="D13">
-        <v>0.3555345617819903</v>
+        <v>0.5168544586054306</v>
       </c>
       <c r="E13">
-        <v>0.7677676499523128</v>
+        <v>0.6998910696304432</v>
       </c>
       <c r="F13">
-        <v>6.47495117760737</v>
+        <v>14.91701268174508</v>
       </c>
       <c r="G13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="H13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="I13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="J13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="K13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="L13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="M13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="N13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
       <c r="O13">
-        <v>-0.05561647331730443</v>
+        <v>0.1428189670628842</v>
       </c>
     </row>
   </sheetData>
@@ -1092,46 +1092,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.3404985380793831</v>
+        <v>0.4737905974083943</v>
       </c>
       <c r="C4">
-        <v>0.3236492621527796</v>
+        <v>0.2251873995317718</v>
       </c>
       <c r="D4">
-        <v>0.816612326943446</v>
+        <v>0.6678741197074448</v>
       </c>
       <c r="E4">
-        <v>0.8992486843170349</v>
+        <v>0.76237658474828</v>
       </c>
       <c r="F4">
-        <v>7.11631654777257</v>
+        <v>6.225763477839968</v>
       </c>
       <c r="G4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="H4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="I4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="J4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="K4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="L4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="M4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="N4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
       <c r="O4">
-        <v>-0.1767951139780164</v>
+        <v>-0.1602939094518714</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1139,46 +1139,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.3891958581353412</v>
+        <v>0.4257095877811176</v>
       </c>
       <c r="C5">
-        <v>0.2098505645987911</v>
+        <v>0.2542622452137207</v>
       </c>
       <c r="D5">
-        <v>0.8446827158465987</v>
+        <v>0.836763666899154</v>
       </c>
       <c r="E5">
-        <v>0.7446006363740362</v>
+        <v>0.6675763281209955</v>
       </c>
       <c r="F5">
-        <v>3.920309885524912</v>
+        <v>5.438303243268854</v>
       </c>
       <c r="G5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="H5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="I5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="J5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="K5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="L5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="M5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="N5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
       <c r="O5">
-        <v>-0.3280323434485395</v>
+        <v>-0.3692730642391807</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1186,46 +1186,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.3647766285496614</v>
+        <v>0.5544505933466822</v>
       </c>
       <c r="C6">
-        <v>0.2672617325075488</v>
+        <v>0.3504960353901989</v>
       </c>
       <c r="D6">
-        <v>0.7629398292744867</v>
+        <v>0.8446462661294293</v>
       </c>
       <c r="E6">
-        <v>0.7953010898418792</v>
+        <v>0.7408158587550198</v>
       </c>
       <c r="F6">
-        <v>11.58213234698223</v>
+        <v>8.479755361918786</v>
       </c>
       <c r="G6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="H6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="I6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="J6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="K6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="L6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="M6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="N6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
       <c r="O6">
-        <v>-0.08576727761679209</v>
+        <v>-0.281508697560007</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1233,46 +1233,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.397692802485008</v>
+        <v>0.313146106694368</v>
       </c>
       <c r="C7">
-        <v>0.3091803690571324</v>
+        <v>0.3161840051583386</v>
       </c>
       <c r="D7">
-        <v>0.6830149595163397</v>
+        <v>0.9579149808442281</v>
       </c>
       <c r="E7">
-        <v>0.6767220319780584</v>
+        <v>0.8423400673436312</v>
       </c>
       <c r="F7">
-        <v>8.845353267439352</v>
+        <v>8.985889819251099</v>
       </c>
       <c r="G7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="H7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="I7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="J7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="K7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="L7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="M7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="N7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
       <c r="O7">
-        <v>-0.06506959985698424</v>
+        <v>-0.1379025875983152</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1280,46 +1280,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.4598475553701047</v>
+        <v>0.4250636975228743</v>
       </c>
       <c r="C8">
-        <v>0.2032479242674561</v>
+        <v>0.2155168622446154</v>
       </c>
       <c r="D8">
-        <v>0.9199982404493721</v>
+        <v>0.8249260835217658</v>
       </c>
       <c r="E8">
-        <v>0.778201008798621</v>
+        <v>0.7434673299640161</v>
       </c>
       <c r="F8">
-        <v>3.130703678760561</v>
+        <v>8.257667614402544</v>
       </c>
       <c r="G8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="H8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="I8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="J8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="K8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="L8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="M8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="N8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
       <c r="O8">
-        <v>-0.4088725084040999</v>
+        <v>-0.218174524247665</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1327,46 +1327,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.4145230477637146</v>
+        <v>0.3207023461129328</v>
       </c>
       <c r="C9">
-        <v>0.3332279073387567</v>
+        <v>0.3252843637804589</v>
       </c>
       <c r="D9">
-        <v>0.8474797462352981</v>
+        <v>0.7279118933234172</v>
       </c>
       <c r="E9">
-        <v>0.7401643063544607</v>
+        <v>0.6875549509510708</v>
       </c>
       <c r="F9">
-        <v>18.89730183370705</v>
+        <v>6.447394692564041</v>
       </c>
       <c r="G9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="H9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="I9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="J9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="K9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="L9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="M9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="N9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
       <c r="O9">
-        <v>0.3738936816160691</v>
+        <v>-0.1834700534751949</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1374,46 +1374,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.3730301435559069</v>
+        <v>0.3965148767660239</v>
       </c>
       <c r="C10">
-        <v>0.2114050728472736</v>
+        <v>0.198368587144049</v>
       </c>
       <c r="D10">
-        <v>0.7653985127840373</v>
+        <v>0.646828564688521</v>
       </c>
       <c r="E10">
-        <v>0.7534390211370979</v>
+        <v>0.684807795356371</v>
       </c>
       <c r="F10">
-        <v>13.65092825240612</v>
+        <v>14.28973054796869</v>
       </c>
       <c r="G10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="H10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="I10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="J10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="K10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="L10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="M10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="N10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
       <c r="O10">
-        <v>0.1481157120954539</v>
+        <v>0.1709226826260663</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1421,46 +1421,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.3785693436802047</v>
+        <v>0.2885255806990877</v>
       </c>
       <c r="C11">
-        <v>0.3371721402770567</v>
+        <v>0.3188088189376265</v>
       </c>
       <c r="D11">
-        <v>0.6264017169442121</v>
+        <v>0.6056918421846318</v>
       </c>
       <c r="E11">
-        <v>0.7661602120379316</v>
+        <v>0.7336240879309854</v>
       </c>
       <c r="F11">
-        <v>7.385832721835889</v>
+        <v>4.00417523891501</v>
       </c>
       <c r="G11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="H11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="I11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="J11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="K11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="L11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="M11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="N11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
       <c r="O11">
-        <v>-0.06902148237131539</v>
+        <v>-0.3262059405783438</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1468,46 +1468,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.2540470619189764</v>
+        <v>0.376975716306263</v>
       </c>
       <c r="C12">
-        <v>0.250001203637881</v>
+        <v>0.3359608556695994</v>
       </c>
       <c r="D12">
-        <v>0.8305448115271902</v>
+        <v>0.7969029059358319</v>
       </c>
       <c r="E12">
-        <v>0.6232225847835118</v>
+        <v>0.8462430478447668</v>
       </c>
       <c r="F12">
-        <v>6.172087277874474</v>
+        <v>15.8374696332879</v>
       </c>
       <c r="G12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="H12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="I12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="J12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="K12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="L12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="M12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="N12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
       <c r="O12">
-        <v>-0.1436852634511429</v>
+        <v>0.03620464884812265</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1515,46 +1515,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.4743048217246052</v>
+        <v>0.3503061845824836</v>
       </c>
       <c r="C13">
-        <v>0.2959430403925805</v>
+        <v>0.2752878387930494</v>
       </c>
       <c r="D13">
-        <v>0.6233774972129159</v>
+        <v>0.8416455517930976</v>
       </c>
       <c r="E13">
-        <v>0.6951953230935235</v>
+        <v>0.7527729850878024</v>
       </c>
       <c r="F13">
-        <v>6.809589567074502</v>
+        <v>8.256595217174857</v>
       </c>
       <c r="G13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="H13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="I13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="J13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="K13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="L13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="M13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="N13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
       <c r="O13">
-        <v>-0.2308484305895594</v>
+        <v>-0.2479972613455617</v>
       </c>
     </row>
   </sheetData>
@@ -1656,46 +1656,46 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.4813036000497379</v>
+        <v>0.4646689007306535</v>
       </c>
       <c r="C4">
-        <v>0.8669464909990061</v>
+        <v>0.8469990113251566</v>
       </c>
       <c r="D4">
-        <v>0.6047327411485997</v>
+        <v>0.6899229991576823</v>
       </c>
       <c r="E4">
-        <v>0.9883575771379397</v>
+        <v>0.9500598239947607</v>
       </c>
       <c r="F4">
-        <v>21.97777617341347</v>
+        <v>33.79909789794387</v>
       </c>
       <c r="G4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="H4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="I4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="J4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="K4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="L4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="M4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="N4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
       <c r="O4">
-        <v>0.08855165436982884</v>
+        <v>0.2638148103843386</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1703,46 +1703,46 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.49281065566889</v>
+        <v>0.5050649953352254</v>
       </c>
       <c r="C5">
-        <v>0.8125204316230247</v>
+        <v>0.8728300584732172</v>
       </c>
       <c r="D5">
-        <v>0.6599481343843909</v>
+        <v>0.6654622740291004</v>
       </c>
       <c r="E5">
-        <v>0.9212110695789697</v>
+        <v>1.015634168756318</v>
       </c>
       <c r="F5">
-        <v>35.09304065811545</v>
+        <v>27.29799585344962</v>
       </c>
       <c r="G5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="H5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="I5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="J5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="K5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="L5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="M5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="N5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
       <c r="O5">
-        <v>0.3468738891874102</v>
+        <v>0.6463715927243818</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1750,46 +1750,46 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>0.5010986894508617</v>
+        <v>0.4812884350615457</v>
       </c>
       <c r="C6">
-        <v>0.8647140272499581</v>
+        <v>0.8785831398011616</v>
       </c>
       <c r="D6">
-        <v>0.627656899670919</v>
+        <v>0.5142657202186506</v>
       </c>
       <c r="E6">
-        <v>0.9683446984132138</v>
+        <v>0.9687815296570539</v>
       </c>
       <c r="F6">
-        <v>38.56710507158374</v>
+        <v>33.44836123433927</v>
       </c>
       <c r="G6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="H6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="I6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="J6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="K6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="L6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="M6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="N6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
       <c r="O6">
-        <v>0.5828316123693374</v>
+        <v>4.333741975303767</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1797,46 +1797,46 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0.5568973137503673</v>
+        <v>0.5361770792856465</v>
       </c>
       <c r="C7">
-        <v>0.859035605326836</v>
+        <v>0.8283041185718691</v>
       </c>
       <c r="D7">
-        <v>0.6717793388374531</v>
+        <v>0.6779778799299384</v>
       </c>
       <c r="E7">
-        <v>0.9861119698266072</v>
+        <v>1.003176571602306</v>
       </c>
       <c r="F7">
-        <v>38.26032941225483</v>
+        <v>49.02694939345981</v>
       </c>
       <c r="G7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="H7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="I7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="J7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="K7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="L7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="M7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="N7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
       <c r="O7">
-        <v>1.254216328613806</v>
+        <v>0.721291060236775</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1844,46 +1844,46 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0.4510100136757352</v>
+        <v>0.4664272292825231</v>
       </c>
       <c r="C8">
-        <v>0.8389653843801657</v>
+        <v>0.8198100070799812</v>
       </c>
       <c r="D8">
-        <v>0.616546371201895</v>
+        <v>0.602296584440869</v>
       </c>
       <c r="E8">
-        <v>0.9891135969256521</v>
+        <v>0.9898257296390327</v>
       </c>
       <c r="F8">
-        <v>26.29207472298372</v>
+        <v>39.30324478023091</v>
       </c>
       <c r="G8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="H8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="I8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="J8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="K8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="L8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="M8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="N8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
       <c r="O8">
-        <v>0.5208117114527848</v>
+        <v>0.07713319628101992</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1891,46 +1891,46 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0.4012507430652762</v>
+        <v>0.5183635346245292</v>
       </c>
       <c r="C9">
-        <v>0.8372111617839993</v>
+        <v>0.8215299163799084</v>
       </c>
       <c r="D9">
-        <v>0.6009484894043411</v>
+        <v>0.6599589466754704</v>
       </c>
       <c r="E9">
-        <v>0.9827482295720914</v>
+        <v>0.9745235193160984</v>
       </c>
       <c r="F9">
-        <v>42.92192830022178</v>
+        <v>40.42362892625581</v>
       </c>
       <c r="G9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="H9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="I9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="J9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="K9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="L9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="M9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="N9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
       <c r="O9">
-        <v>0.6147259615237898</v>
+        <v>1.111620295182078</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1938,46 +1938,46 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>0.533681084688559</v>
+        <v>0.4564130489891881</v>
       </c>
       <c r="C10">
-        <v>0.7995682964875506</v>
+        <v>0.8191057191728001</v>
       </c>
       <c r="D10">
-        <v>0.6236034439428224</v>
+        <v>0.5143168259235524</v>
       </c>
       <c r="E10">
-        <v>0.982711461085473</v>
+        <v>0.9689962922173687</v>
       </c>
       <c r="F10">
-        <v>34.18852041523162</v>
+        <v>44.1534544496569</v>
       </c>
       <c r="G10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="H10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="I10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="J10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="K10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="L10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="M10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="N10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
       <c r="O10">
-        <v>0.1770869208847956</v>
+        <v>1.316124349342227</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1985,46 +1985,46 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.5339219698899847</v>
+        <v>0.4390534008167248</v>
       </c>
       <c r="C11">
-        <v>0.8261299281310026</v>
+        <v>0.7990643497315116</v>
       </c>
       <c r="D11">
-        <v>0.57526470341659</v>
+        <v>0.481379429912202</v>
       </c>
       <c r="E11">
-        <v>0.9531485199903575</v>
+        <v>0.9174453287291314</v>
       </c>
       <c r="F11">
-        <v>69.83362817448757</v>
+        <v>29.03579993797534</v>
       </c>
       <c r="G11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="H11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="I11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="J11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="K11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="L11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="M11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="N11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
       <c r="O11">
-        <v>6.301488134964102</v>
+        <v>0.6994478314582776</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -2032,46 +2032,46 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>0.51853711896593</v>
+        <v>0.495071415624479</v>
       </c>
       <c r="C12">
-        <v>0.8710800683111276</v>
+        <v>0.798228516208398</v>
       </c>
       <c r="D12">
-        <v>0.6264029431560781</v>
+        <v>0.6509569139113891</v>
       </c>
       <c r="E12">
-        <v>1.032854135276037</v>
+        <v>0.9687090020368436</v>
       </c>
       <c r="F12">
-        <v>31.94571874549643</v>
+        <v>43.23108821908976</v>
       </c>
       <c r="G12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="H12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="I12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="J12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="K12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="L12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="M12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="N12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
       <c r="O12">
-        <v>3.42947309439512</v>
+        <v>2.351743922022746</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2079,46 +2079,46 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>0.4066424522202957</v>
+        <v>0.4957144739317061</v>
       </c>
       <c r="C13">
-        <v>0.8159884965488076</v>
+        <v>0.884116264932801</v>
       </c>
       <c r="D13">
-        <v>0.4871506396883109</v>
+        <v>0.601985465309452</v>
       </c>
       <c r="E13">
-        <v>0.9714380511667401</v>
+        <v>0.9736631530539833</v>
       </c>
       <c r="F13">
-        <v>41.88085624618613</v>
+        <v>28.51847984702074</v>
       </c>
       <c r="G13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="H13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="I13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="J13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="K13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="L13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="M13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="N13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
       <c r="O13">
-        <v>1.685553353225906</v>
+        <v>0.299668837038222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>